<commit_message>
step one finished auto gen from template
</commit_message>
<xml_diff>
--- a/parameters_XLS_3_bottom_plate_boven.xlsx
+++ b/parameters_XLS_3_bottom_plate_boven.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PYHTON\xeryon_auto_cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73EBB402-D0F0-4686-9F86-4774A505A7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9B7005-D738-4CDC-8520-71E54A5A9FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="66900" yWindow="0" windowWidth="13845" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Param" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
   <si>
     <t>twee keer -25 bij vacuum groef 80…</t>
   </si>
@@ -63,64 +63,184 @@
     <t>COLUMNS</t>
   </si>
   <si>
-    <t>USES_PATROON 42 X 39 MM</t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
     <t>YES</t>
   </si>
   <si>
-    <t>FOR_EINDESLAG_X</t>
-  </si>
-  <si>
-    <t>[-7,-4.5,-2,2,4.5,7]</t>
-  </si>
-  <si>
-    <t>[-17,-9.5,-7,-3,3,7,9.5,17]</t>
-  </si>
-  <si>
-    <t>[-12,-8,-2.5,2.5,8,12]</t>
-  </si>
-  <si>
-    <t>[-12,-7,-2.5,2.5,7,12]</t>
-  </si>
-  <si>
-    <t>FOR_COUNTERBORE_M2</t>
-  </si>
-  <si>
-    <t>[-15,-5,5,15]</t>
-  </si>
-  <si>
-    <t>[-35,-25,-15,-5,5,15,25,35]</t>
-  </si>
-  <si>
-    <t>EINDELOOP</t>
-  </si>
-  <si>
-    <t>SLEUF_EINDESLAG_X</t>
-  </si>
-  <si>
-    <t>1103_040_002_G2_BOVEN</t>
-  </si>
-  <si>
-    <t>1103_060_002_G2_BOVEN</t>
-  </si>
-  <si>
-    <t>1103_080_002_G2_BOVEN</t>
-  </si>
-  <si>
-    <t>1103_120_002_G2_BOVEN</t>
-  </si>
-  <si>
-    <t>[-25,-15,-5,5,15,25]</t>
-  </si>
-  <si>
-    <t>SPANKLEMMEN</t>
-  </si>
-  <si>
-    <t>[-55,-45,-35,-25,-15,-5,5,15,25,35,45,55]</t>
+    <t>1103_040_001_G8_BOVEN</t>
+  </si>
+  <si>
+    <t>1103_060_001_G8_BOVEN</t>
+  </si>
+  <si>
+    <t>1103_080_001_G8_BOVEN</t>
+  </si>
+  <si>
+    <t>1103_120_001_G8_BOVEN</t>
+  </si>
+  <si>
+    <t>PILOOT_X1</t>
+  </si>
+  <si>
+    <t>PILOOT_X2</t>
+  </si>
+  <si>
+    <t>PILOOT_X3</t>
+  </si>
+  <si>
+    <t>PILOOT_X4</t>
+  </si>
+  <si>
+    <t>PILOOT_Y1</t>
+  </si>
+  <si>
+    <t>PILOOT_Y2</t>
+  </si>
+  <si>
+    <t>PILOOT_Y3</t>
+  </si>
+  <si>
+    <t>PILOOT_Y4</t>
+  </si>
+  <si>
+    <t>25.8</t>
+  </si>
+  <si>
+    <t>USES_COUNTERBORE_D5.5</t>
+  </si>
+  <si>
+    <t>2.2_AFST</t>
+  </si>
+  <si>
+    <t>2.2_COLUMNS</t>
+  </si>
+  <si>
+    <t>2.5_COLUMNS</t>
+  </si>
+  <si>
+    <t>USES_STATOR_MASS_COMP</t>
+  </si>
+  <si>
+    <t>3.2_COLUMNS</t>
+  </si>
+  <si>
+    <t>3.2_AFST</t>
+  </si>
+  <si>
+    <t>USES_EXTRA_CABLE</t>
+  </si>
+  <si>
+    <t>3.5_COLUMNS</t>
+  </si>
+  <si>
+    <t>USES_2.9_MM_BEVEST</t>
+  </si>
+  <si>
+    <t>FOR_VACUUM_GROEF_X</t>
+  </si>
+  <si>
+    <t>[-10,-5,5,10,15]</t>
+  </si>
+  <si>
+    <t>[-30,-25,-20,-15,-10,-5,5,10,15,20,25,30,35]</t>
+  </si>
+  <si>
+    <t>USES_COORD</t>
+  </si>
+  <si>
+    <t>SELECT_FIJNBEWERKING</t>
+  </si>
+  <si>
+    <t>USES_MOTOR_VERZINKING</t>
+  </si>
+  <si>
+    <t>TAP_DIST</t>
+  </si>
+  <si>
+    <t>COLUMNS_7.4</t>
+  </si>
+  <si>
+    <t>SELECT_LABELS</t>
+  </si>
+  <si>
+    <t>-25.8</t>
+  </si>
+  <si>
+    <t>USES_IDK</t>
+  </si>
+  <si>
+    <t>labels_xls_3_40_bottom_plate_boven.H</t>
+  </si>
+  <si>
+    <t>labels_xls_3_60_bottom_plate_boven.H</t>
+  </si>
+  <si>
+    <t>labels_xls_3_80_bottom_plate_boven.H</t>
+  </si>
+  <si>
+    <t>labels_xls_3_120_bottom_plate_boven.H</t>
+  </si>
+  <si>
+    <t>fijnbewerking_xls_3_40_bottom_plate_boven.H</t>
+  </si>
+  <si>
+    <t>fijnbewerking_xls_3_60_bottom_plate_boven.H</t>
+  </si>
+  <si>
+    <t>fijnbewerking_xls_3_80_bottom_plate_boven.H</t>
+  </si>
+  <si>
+    <t>fijnbewerking_xls_3_120_bottom_plate_boven.H</t>
+  </si>
+  <si>
+    <t>2.2_AFST_B</t>
+  </si>
+  <si>
+    <t>2.2_START</t>
+  </si>
+  <si>
+    <t>2.5_START</t>
+  </si>
+  <si>
+    <t>2.5_AFST</t>
+  </si>
+  <si>
+    <t>3.2_AFST_B</t>
+  </si>
+  <si>
+    <t>3.2_START</t>
+  </si>
+  <si>
+    <t>3.5_START</t>
+  </si>
+  <si>
+    <t>3.5_AFST</t>
+  </si>
+  <si>
+    <t>[-20,-15,-10,-5,5,10,15,20,25]</t>
+  </si>
+  <si>
+    <t>7.2_START</t>
+  </si>
+  <si>
+    <t>7.2_AFST</t>
+  </si>
+  <si>
+    <t>7.4_AFST</t>
+  </si>
+  <si>
+    <t>USES_PATROON 44 X 30 MM</t>
+  </si>
+  <si>
+    <t>VACUUM_GROEF_START</t>
+  </si>
+  <si>
+    <t>7.2_COORD</t>
+  </si>
+  <si>
+    <t>[-50,-45,-40,-35,-30,-25,-20,-15,-10,-5,5,10,15,20,25,30,35,40,45,50,55]</t>
   </si>
 </sst>
 </file>
@@ -130,7 +250,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +292,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -221,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -256,8 +382,11 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -564,16 +693,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="27.26171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="22.5234375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.3671875" customWidth="1"/>
+    <col min="2" max="3" width="22.5234375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.3125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.9453125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="13.578125" bestFit="1" customWidth="1"/>
@@ -602,164 +732,772 @@
         <v>6</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B3" s="7">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="C3" s="7">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="D3" s="7">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="E3" s="7">
-        <v>6</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="7">
-        <v>40</v>
+        <v>15</v>
+      </c>
+      <c r="B4" s="12">
+        <v>-22</v>
       </c>
       <c r="C4" s="7">
-        <v>60</v>
+        <v>-32</v>
       </c>
       <c r="D4" s="7">
-        <v>80</v>
+        <v>-27</v>
       </c>
       <c r="E4" s="7">
-        <v>120</v>
+        <v>-37</v>
       </c>
       <c r="I4" s="9"/>
     </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>28</v>
+        <v>16</v>
+      </c>
+      <c r="B5" s="7">
+        <v>22</v>
+      </c>
+      <c r="C5" s="7">
+        <v>32</v>
+      </c>
+      <c r="D5" s="7">
+        <v>-27</v>
+      </c>
+      <c r="E5" s="7">
+        <v>-37</v>
       </c>
       <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="8">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="C6" s="8">
-        <v>38.4</v>
-      </c>
-      <c r="D6" s="8">
-        <v>28.4</v>
-      </c>
-      <c r="E6" s="8">
-        <v>28.4</v>
+        <v>17</v>
+      </c>
+      <c r="B6" s="7">
+        <v>-22</v>
+      </c>
+      <c r="C6" s="7">
+        <v>-32</v>
+      </c>
+      <c r="D6" s="7">
+        <v>-33</v>
+      </c>
+      <c r="E6" s="7">
+        <v>-43</v>
       </c>
       <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="11">
-        <f>B4/10</f>
-        <v>4</v>
-      </c>
-      <c r="C7" s="11">
-        <f>C4/10</f>
-        <v>6</v>
-      </c>
-      <c r="D7" s="11">
-        <f>D4/10</f>
-        <v>8</v>
-      </c>
-      <c r="E7" s="11">
-        <f>E4/10</f>
-        <v>12</v>
+      <c r="A7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="7">
+        <v>22</v>
+      </c>
+      <c r="C7" s="7">
+        <v>32</v>
+      </c>
+      <c r="D7" s="7">
+        <v>33</v>
+      </c>
+      <c r="E7" s="7">
+        <v>43</v>
       </c>
       <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>11</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B8" s="7">
+        <v>20</v>
+      </c>
+      <c r="C8" s="7">
+        <v>20</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="9"/>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>20</v>
+      </c>
+      <c r="B9" s="7">
+        <v>-20</v>
+      </c>
+      <c r="C9" s="7">
+        <v>-20</v>
+      </c>
+      <c r="D9" s="8">
+        <v>-25.8</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="12">
-        <v>7</v>
-      </c>
-      <c r="C10" s="12">
-        <v>17</v>
-      </c>
-      <c r="D10" s="12">
+      <c r="B10" s="7">
+        <v>-15</v>
+      </c>
+      <c r="C10" s="7">
+        <v>-15</v>
+      </c>
+      <c r="D10" s="8">
+        <v>-25.8</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="7">
+        <v>15</v>
+      </c>
+      <c r="C11" s="7">
+        <v>15</v>
+      </c>
+      <c r="D11" s="8">
+        <v>-25.8</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="6" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="11">
+        <v>4</v>
+      </c>
+      <c r="C14" s="11">
+        <v>6</v>
+      </c>
+      <c r="D14" s="11">
+        <v>8</v>
+      </c>
+      <c r="E14" s="11">
         <v>12</v>
       </c>
-      <c r="E10" s="12">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="E13" s="5"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="11">
+        <v>0</v>
+      </c>
+      <c r="C15" s="11">
+        <v>20</v>
+      </c>
+      <c r="D15" s="11">
+        <v>-20</v>
+      </c>
+      <c r="E15" s="11">
+        <v>20</v>
+      </c>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="11">
+        <v>10</v>
+      </c>
+      <c r="C16" s="11">
+        <v>-20</v>
+      </c>
+      <c r="D16" s="11">
+        <v>10</v>
+      </c>
+      <c r="E16" s="11">
+        <v>-50</v>
+      </c>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="11">
+        <v>0</v>
+      </c>
+      <c r="C17" s="11">
+        <v>40</v>
+      </c>
+      <c r="D17" s="11">
+        <v>20</v>
+      </c>
+      <c r="E17" s="11">
+        <v>100</v>
+      </c>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="11">
+        <v>1</v>
+      </c>
+      <c r="C18" s="11">
+        <v>2</v>
+      </c>
+      <c r="D18" s="11">
+        <v>2</v>
+      </c>
+      <c r="E18" s="11">
+        <v>2</v>
+      </c>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="11">
+        <v>-10</v>
+      </c>
+      <c r="C19" s="11">
+        <v>-20</v>
+      </c>
+      <c r="D19" s="11">
+        <v>-10</v>
+      </c>
+      <c r="E19" s="11">
+        <v>-50</v>
+      </c>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="11">
+        <v>-10</v>
+      </c>
+      <c r="C20" s="11">
+        <v>10</v>
+      </c>
+      <c r="D20" s="11">
+        <v>-10</v>
+      </c>
+      <c r="E20" s="11">
+        <v>10</v>
+      </c>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="11">
+        <v>1</v>
+      </c>
+      <c r="C21" s="11">
+        <v>2</v>
+      </c>
+      <c r="D21" s="11">
+        <v>3</v>
+      </c>
+      <c r="E21" s="11">
+        <v>5</v>
+      </c>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="11">
+        <v>10</v>
+      </c>
+      <c r="C23" s="11">
+        <v>-20</v>
+      </c>
+      <c r="D23" s="11">
+        <v>10</v>
+      </c>
+      <c r="E23" s="11">
+        <v>-50</v>
+      </c>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="11">
+        <v>1</v>
+      </c>
+      <c r="C24" s="11">
+        <v>2</v>
+      </c>
+      <c r="D24" s="11">
+        <v>2</v>
+      </c>
+      <c r="E24" s="11">
+        <v>2</v>
+      </c>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="11">
+        <v>0</v>
+      </c>
+      <c r="C25" s="11">
+        <v>20</v>
+      </c>
+      <c r="D25" s="11">
+        <v>-20</v>
+      </c>
+      <c r="E25" s="11">
+        <v>20</v>
+      </c>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="11">
+        <v>0</v>
+      </c>
+      <c r="C26" s="11">
+        <v>40</v>
+      </c>
+      <c r="D26" s="11">
+        <v>20</v>
+      </c>
+      <c r="E26" s="11">
+        <v>100</v>
+      </c>
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="11">
+        <v>-10</v>
+      </c>
+      <c r="C28" s="11">
+        <v>-20</v>
+      </c>
+      <c r="D28" s="11">
+        <v>-10</v>
+      </c>
+      <c r="E28" s="11">
+        <v>-50</v>
+      </c>
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="11">
+        <v>-10</v>
+      </c>
+      <c r="C29" s="11">
+        <v>10</v>
+      </c>
+      <c r="D29" s="11">
+        <v>-10</v>
+      </c>
+      <c r="E29" s="11">
+        <v>10</v>
+      </c>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="11">
+        <v>1</v>
+      </c>
+      <c r="C30" s="11">
+        <v>2</v>
+      </c>
+      <c r="D30" s="11">
+        <v>2</v>
+      </c>
+      <c r="E30" s="11">
+        <v>5</v>
+      </c>
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="11">
+        <v>-15</v>
+      </c>
+      <c r="C32" s="11">
+        <v>-25</v>
+      </c>
+      <c r="D32" s="11">
+        <v>-15</v>
+      </c>
+      <c r="E32" s="11">
+        <v>-55</v>
+      </c>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="11">
+        <v>-20</v>
+      </c>
+      <c r="C35" s="11">
+        <v>-20</v>
+      </c>
+      <c r="D35" s="11">
+        <v>-30</v>
+      </c>
+      <c r="E35" s="11">
+        <v>-50</v>
+      </c>
+      <c r="I35" s="9"/>
+    </row>
+    <row r="36" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="11">
+        <v>0</v>
+      </c>
+      <c r="C39" s="11">
+        <v>-20</v>
+      </c>
+      <c r="D39" s="11">
+        <v>20</v>
+      </c>
+      <c r="E39" s="11">
+        <v>-20</v>
+      </c>
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="11">
+        <v>10</v>
+      </c>
+      <c r="C40" s="11">
+        <v>-20</v>
+      </c>
+      <c r="D40" s="11">
+        <v>10</v>
+      </c>
+      <c r="E40" s="11">
+        <v>-50</v>
+      </c>
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="11">
+        <v>0</v>
+      </c>
+      <c r="C41" s="11">
+        <v>40</v>
+      </c>
+      <c r="D41" s="11">
+        <v>20</v>
+      </c>
+      <c r="E41" s="11">
+        <v>100</v>
+      </c>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="11">
+        <v>1</v>
+      </c>
+      <c r="C42" s="11">
+        <v>2</v>
+      </c>
+      <c r="D42" s="11">
+        <v>3</v>
+      </c>
+      <c r="E42" s="11">
+        <v>5</v>
+      </c>
+      <c r="I42" s="9"/>
+    </row>
+    <row r="43" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="11">
+        <v>-10</v>
+      </c>
+      <c r="C43" s="11">
+        <v>10</v>
+      </c>
+      <c r="D43" s="11">
+        <v>10</v>
+      </c>
+      <c r="E43" s="11">
+        <v>10</v>
+      </c>
+      <c r="I43" s="9"/>
+    </row>
+    <row r="44" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I44" s="9"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="E47" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>